<commit_message>
Updated the SRC Files
</commit_message>
<xml_diff>
--- a/src/test/resources/Coordinates.xlsx
+++ b/src/test/resources/Coordinates.xlsx
@@ -5,26 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akilesh Nagarajan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akilesh Nagarajan\eclipse-workspace\API_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD1DB17-8459-4208-AB81-B92C858AF0EC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B789246E-E576-4C89-8B65-4684183D4CA9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8520" yWindow="2325" windowWidth="21600" windowHeight="12195" xr2:uid="{EFE4511B-B9CD-455D-843F-032C718F6130}"/>
+    <workbookView xWindow="8295" yWindow="2010" windowWidth="21600" windowHeight="12195" xr2:uid="{EFE4511B-B9CD-455D-843F-032C718F6130}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -72,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC70D848-3D76-43A9-887C-8E252E7741B3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,22 +406,79 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>40.730609999999999</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>-73.935242000000002</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
+        <v>35.772100000000002</v>
+      </c>
+      <c r="B3" s="1">
+        <v>-78.63861</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>38.122999999999998</v>
       </c>
-      <c r="B3">
+      <c r="B4" s="1">
         <v>-78.543000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>35.600960000000001</v>
+      </c>
+      <c r="B5" s="1">
+        <v>-81.646708666666697</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>34.297154999999997</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-83.950587666666706</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>32.99335</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-86.254466666666701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>31.689544999999999</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-88.558345666666696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>30.385739999999998</v>
+      </c>
+      <c r="B9" s="1">
+        <v>-90.862224666666705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>29.081935000000001</v>
+      </c>
+      <c r="B10" s="1">
+        <v>-93.1661036666667</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>